<commit_message>
fixed #44 TournRPG-44 ダイアログの実装
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>防御力</t>
+  </si>
+  <si>
+    <t>はい</t>
+  </si>
+  <si>
+    <t>いいえ</t>
+  </si>
+  <si>
+    <t>アイテムを捨てて&lt;val1&gt;を手に入れますか？</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1615,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1635,7 +1644,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
-        <f t="shared" si="0" ref="A3:A4">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A7">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -1643,12 +1652,39 @@
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s" s="4">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #31 TournRPG-31 レベルアップの実装
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>&lt;val1&gt;の経験値を獲得した</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;はレベルアップした</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;はHPが全回復した</t>
   </si>
   <si>
     <t>攻撃力</t>
@@ -1487,7 +1493,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1523,7 +1529,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
-        <f t="shared" si="0" ref="A3:A18">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A20">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -1711,6 +1717,30 @@
       </c>
       <c r="C18" t="s" s="4">
         <v>15</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1">
+      <c r="A19" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s" s="4">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1">
+      <c r="A20" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s" s="4">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s" s="4">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1760,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -1769,7 +1799,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -1778,7 +1808,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -1787,7 +1817,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -1796,7 +1826,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -1805,7 +1835,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #64 TournRPG-64 攻撃スキルを作る
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -99,6 +99,9 @@
     <t>&lt;val1&gt;はHPが全回復した</t>
   </si>
   <si>
+    <t>&lt;val1&gt;は&lt;val2&gt;を発動した</t>
+  </si>
+  <si>
     <t>攻撃力</t>
   </si>
   <si>
@@ -115,6 +118,15 @@
   </si>
   <si>
     <t>キャンセル</t>
+  </si>
+  <si>
+    <t>攻撃</t>
+  </si>
+  <si>
+    <t>アイテム</t>
+  </si>
+  <si>
+    <t>逃走</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1505,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1529,7 +1541,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
-        <f t="shared" si="0" ref="A3:A20">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A21">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -1741,6 +1753,18 @@
       </c>
       <c r="C20" t="s" s="4">
         <v>17</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="A21" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s" s="4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1757,7 +1781,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1786,11 +1810,11 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
-        <f t="shared" si="0" ref="A3:A8">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A11">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -1799,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -1808,7 +1832,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -1817,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -1826,16 +1850,43 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1">
+      <c r="A11" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s" s="4">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #187 TournRPG-187 メニューボタンの実装
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>敵全体</t>
+  </si>
+  <si>
+    <t>メニュー</t>
   </si>
 </sst>
 </file>
@@ -2042,7 +2045,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2071,7 +2074,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
-        <f t="shared" si="0" ref="A3:A12">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A13">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2151,12 +2154,21 @@
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
-      <c r="A12" s="6">
+      <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>56</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s" s="4">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #189 TournRPG-189 バフのメッセージ表示
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>&lt;val1&gt;は痺れて動けない</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;の攻撃力がアップした</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;の防御力力がアップした</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;の素早さがアップした</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;の攻撃力がダウンした</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;の防御力力がダウンした</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;の素早さがダウンした</t>
   </si>
   <si>
     <t>攻撃力</t>
@@ -1565,7 +1583,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1601,7 +1619,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="3">
-        <f t="shared" si="0" ref="A3:A38">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A44">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2029,6 +2047,78 @@
       </c>
       <c r="C38" t="s" s="4">
         <v>10</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1">
+      <c r="A39" s="3">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s" s="4">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1">
+      <c r="A40" s="3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" ht="20" customHeight="1">
+      <c r="A41" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s" s="4">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1">
+      <c r="A42" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" t="s" s="4">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="A43" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s" s="4">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1">
+      <c r="A44" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" t="s" s="4">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s" s="4">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2078,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2087,7 +2177,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2096,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2105,7 +2195,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2114,7 +2204,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2123,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2132,7 +2222,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2141,7 +2231,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2150,7 +2240,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2159,7 +2249,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2168,7 +2258,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #239 TournRPG-239 アイテムを捨てる
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -180,6 +180,9 @@
     <t>&lt;val1&gt;を&lt;val2&gt;Gで売却した</t>
   </si>
   <si>
+    <t>&lt;val1&gt;を捨てた</t>
+  </si>
+  <si>
     <t>攻撃力</t>
   </si>
   <si>
@@ -229,6 +232,9 @@
   </si>
   <si>
     <t>スキル確認</t>
+  </si>
+  <si>
+    <t>アイテム捨てる</t>
   </si>
 </sst>
 </file>
@@ -1448,7 +1454,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1484,7 +1490,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A46">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A47">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2008,6 +2014,18 @@
       </c>
       <c r="C46" t="s" s="4">
         <v>8</v>
+      </c>
+    </row>
+    <row r="47" ht="20" customHeight="1">
+      <c r="A47" s="5">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B47" t="s" s="4">
+        <v>55</v>
+      </c>
+      <c r="C47" t="s" s="4">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2042,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2053,11 +2071,11 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A19">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A20">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2066,7 +2084,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2075,7 +2093,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2084,7 +2102,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2093,7 +2111,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2102,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2111,7 +2129,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2120,7 +2138,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2129,7 +2147,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2138,7 +2156,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2147,7 +2165,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -2156,7 +2174,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -2165,7 +2183,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -2174,7 +2192,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -2183,7 +2201,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -2192,7 +2210,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2201,7 +2219,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>71</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1">
+      <c r="A20" s="5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s" s="4">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #277 TournRPG-277 ショップで回復
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>魔力</t>
+  </si>
+  <si>
+    <t>回復</t>
+  </si>
+  <si>
+    <t>10％回復</t>
+  </si>
+  <si>
+    <t>全回復</t>
   </si>
 </sst>
 </file>
@@ -2132,7 +2141,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2161,7 +2170,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A25">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A28">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2364,6 +2373,33 @@
       </c>
       <c r="B25" t="s" s="4">
         <v>83</v>
+      </c>
+    </row>
+    <row r="26" ht="20" customHeight="1">
+      <c r="A26" s="5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1">
+      <c r="A27" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1">
+      <c r="A28" s="5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s" s="4">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #292 TournRPG-292 HP回復メッセージ詳細
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>id</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>HP全回復</t>
+  </si>
+  <si>
+    <t>HPを10%回復します</t>
+  </si>
+  <si>
+    <t>HPを最大値まで回復します</t>
   </si>
 </sst>
 </file>
@@ -2153,7 +2159,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2182,7 +2188,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A28">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A30">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2412,6 +2418,24 @@
       </c>
       <c r="B28" t="s" s="4">
         <v>86</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1">
+      <c r="A29" s="5">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="A30" s="5">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s" s="4">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #300 TournRPG-300 ターン終了時にHP自動回復
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>&lt;val1&gt;の魔力が&lt;val2&gt;上昇した</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;のMPが&lt;val2&gt;回復した</t>
   </si>
   <si>
     <t>攻撃力</t>
@@ -2139,7 +2142,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s" s="4">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s" s="4">
         <v>18</v>
@@ -2192,7 +2195,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2201,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2210,7 +2213,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2219,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2228,7 +2231,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2237,7 +2240,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2246,7 +2249,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2255,7 +2258,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2264,7 +2267,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2273,7 +2276,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2282,7 +2285,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -2291,7 +2294,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -2300,7 +2303,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -2309,7 +2312,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -2318,7 +2321,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -2327,7 +2330,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2336,7 +2339,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -2345,7 +2348,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -2354,7 +2357,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -2363,7 +2366,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -2372,7 +2375,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -2381,7 +2384,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -2390,7 +2393,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -2399,7 +2402,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -2408,7 +2411,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -2417,7 +2420,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -2426,7 +2429,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -2435,7 +2438,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #321 TournRPG-321 食糧の文字をNumberに移行する
</commit_message>
<xml_diff>
--- a/docs/message.xlsx
+++ b/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>id</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>HPを最大値まで回復します</t>
+  </si>
+  <si>
+    <t>食糧</t>
+  </si>
+  <si>
+    <t>食糧がなくなるとダメージを受けます</t>
   </si>
 </sst>
 </file>
@@ -2162,7 +2168,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2191,7 +2197,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A30">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A32">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2439,6 +2445,24 @@
       </c>
       <c r="B30" t="s" s="4">
         <v>89</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1">
+      <c r="A31" s="5">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1">
+      <c r="A32" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s" s="4">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>